<commit_message>
modify hlm model to resolve single matrix issue
</commit_message>
<xml_diff>
--- a/data/hlm/hlm_train_data.xlsx
+++ b/data/hlm/hlm_train_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E63914A-3251-4B09-ACC6-54A2CFAFC8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853297BA-AC96-4CC1-9F30-62995E28BF0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="732" windowWidth="13068" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3468" yWindow="288" windowWidth="14700" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="erosion" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>

</xml_diff>